<commit_message>
added 11, 153, 190, 268, 33, 338, 371
</commit_message>
<xml_diff>
--- a/leetCodeTeamBlind.xlsx
+++ b/leetCodeTeamBlind.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Competitive_Programming&amp;Job_Prep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Competitive_Programming&amp;Job_Prep\LeetcodePrep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -657,7 +657,7 @@
   <dimension ref="A2:C88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -713,7 +713,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -724,7 +724,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -735,7 +735,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -746,7 +746,7 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -757,7 +757,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
@@ -768,7 +768,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -779,7 +779,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
@@ -790,7 +790,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
@@ -806,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
@@ -817,7 +817,7 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -828,7 +828,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -839,7 +839,7 @@
         <v>25</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
@@ -850,7 +850,7 @@
         <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
added 213, 55, 62, 91,
</commit_message>
<xml_diff>
--- a/leetCodeTeamBlind.xlsx
+++ b/leetCodeTeamBlind.xlsx
@@ -656,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.4"/>
@@ -943,7 +943,7 @@
         <v>33</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
@@ -954,7 +954,7 @@
         <v>34</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
@@ -965,7 +965,7 @@
         <v>35</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
@@ -976,7 +976,7 @@
         <v>36</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">

</xml_diff>